<commit_message>
chore: update input files cells inner paths
Update input file paths to fix error message that appears when they are opened.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_coupling.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_coupling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{50FE14B6-81BC-4FB8-AEBE-71B07C325E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E1C41B-726E-4B60-8C03-69E6713C5B79}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{50FE14B6-81BC-4FB8-AEBE-71B07C325E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D65F672-4C8D-4C45-8CCF-CC30AB7C78E3}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" tabRatio="663" firstSheet="4" activeTab="6" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
+    <workbookView xWindow="29940" yWindow="1215" windowWidth="14400" windowHeight="7365" tabRatio="663" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_perimeter_flag" sheetId="8" r:id="rId1"/>
@@ -612,8 +612,8 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CHAN"/>
+      <sheetName val="STACK"/>
       <sheetName val="STR_MIX"/>
-      <sheetName val="STR_SC"/>
       <sheetName val="STR_STAB"/>
       <sheetName val="Z_JACKET"/>
     </sheetNames>
@@ -628,15 +628,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
         <row r="3">
           <cell r="E3" t="str">
             <v>STR_MIX_1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4">
         <row r="3">
           <cell r="E3" t="str">
@@ -948,31 +948,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631F8432-32B0-4782-8A41-3C8B7D94A95A}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:AB1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>[1]CHAN!$E$3</f>
+        <f>[1]CHAN!E$3</f>
         <v>CHAN_1</v>
       </c>
       <c r="D2" s="5" t="str">
@@ -980,15 +980,15 @@
         <v>CHAN_2</v>
       </c>
       <c r="E2" s="5" t="str">
-        <f>[1]STR_MIX!$E$3</f>
+        <f>[1]STR_MIX!E$3</f>
         <v>STR_MIX_1</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>[1]Z_JACKET!$E$3</f>
+        <f>[1]Z_JACKET!E$3</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -1030,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -1118,21 +1118,21 @@
       <selection activeCell="A8" sqref="A8:XFD109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -1155,7 +1155,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -1176,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -1239,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -1306,20 +1306,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
@@ -1341,7 +1341,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -1457,24 +1457,24 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
@@ -1496,7 +1496,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -1562,7 +1562,7 @@
         <v>9.4355999999999995E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -1584,7 +1584,7 @@
         <v>3.1452000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -1763,19 +1763,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="103.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="15" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -1806,7 +1806,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -1869,7 +1869,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -1890,7 +1890,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -2075,21 +2075,21 @@
       <selection activeCell="G1" sqref="G1:AP1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -2112,7 +2112,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -2175,7 +2175,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -2196,7 +2196,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -2375,21 +2375,21 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -2412,7 +2412,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -2433,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -2454,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -2475,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -2496,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -2675,20 +2675,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
@@ -2710,7 +2710,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -2731,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -2794,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -2825,24 +2825,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC21CE9-E767-48C8-97C0-B436E3F8B9DC}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
@@ -2864,7 +2864,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -2948,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -2982,22 +2982,22 @@
       <selection activeCell="G1" sqref="G1:AH1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -3020,7 +3020,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -3041,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -3063,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
@@ -3171,21 +3171,21 @@
       <selection activeCell="A8" sqref="A8:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="str">
         <f>contact_perimeter_flag!B2</f>
@@ -3208,7 +3208,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="str">
         <f>B2</f>
         <v>Environment</v>
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
@@ -3250,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>

</xml_diff>

<commit_message>
feat!: update input file coductor_coupling.xlsx
Updated input file coductor_coupling.xlsx to introduce variable conductive heat transfer coefficient between solid components.

BREAKING CHANGES

    * new sheet thermal_contact_resistance in input file conductor_coupling.xlsx
    * sheet interface_thickness in file conductro_coupling.xlsx is not only valid for Fluid Components but is valid for all conductor components, including Environment
    * matrix in sheet interface_thickness of file conductro_coupling.xlsx should be fully filled, with the exception of the main diagonal, since matrix in the general case is no loger symmetric.

modified:   input_files/input_file_template/template_conductor_1_coupling.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_coupling.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_coupling.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{50FE14B6-81BC-4FB8-AEBE-71B07C325E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D65F672-4C8D-4C45-8CCF-CC30AB7C78E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A3132-DA30-4CCD-B32D-01E2071A68DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1215" windowWidth="14400" windowHeight="7365" tabRatio="663" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="663" firstSheet="5" activeTab="9" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_perimeter_flag" sheetId="8" r:id="rId1"/>
     <sheet name="contact_perimeter" sheetId="1" r:id="rId2"/>
     <sheet name="HTC_choice" sheetId="4" r:id="rId3"/>
     <sheet name="contact_HTC" sheetId="2" r:id="rId4"/>
-    <sheet name="HTC_multiplier" sheetId="5" r:id="rId5"/>
-    <sheet name="electric_conductance_mode" sheetId="10" r:id="rId6"/>
-    <sheet name="electric_conductance" sheetId="11" r:id="rId7"/>
-    <sheet name="open_perimeter_fract" sheetId="3" r:id="rId8"/>
-    <sheet name="interf_thickness" sheetId="7" r:id="rId9"/>
-    <sheet name="trans_transp_multiplier" sheetId="6" r:id="rId10"/>
-    <sheet name="view_factors" sheetId="9" r:id="rId11"/>
+    <sheet name="thermal_contact_resistance" sheetId="12" r:id="rId5"/>
+    <sheet name="HTC_multiplier" sheetId="5" r:id="rId6"/>
+    <sheet name="electric_conductance_mode" sheetId="10" r:id="rId7"/>
+    <sheet name="electric_conductance" sheetId="11" r:id="rId8"/>
+    <sheet name="open_perimeter_fract" sheetId="3" r:id="rId9"/>
+    <sheet name="interf_thickness" sheetId="7" r:id="rId10"/>
+    <sheet name="trans_transp_multiplier" sheetId="6" r:id="rId11"/>
+    <sheet name="view_factors" sheetId="9" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,15 +47,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>[%] Fraction of the contact perimeter between fluid elements which is actually open</t>
   </si>
   <si>
     <t>[%] Multiplier for the transport properties in the open fraction of the perimeter between fluid elements</t>
-  </si>
-  <si>
-    <t>[m] Thickness of the interface between fluid elements</t>
   </si>
   <si>
     <t>% [W/m2K] Value for the heat transfer coefficient, if constant</t>
@@ -82,6 +80,12 @@
   </si>
   <si>
     <t>[S/m] Value of the electric_conductance</t>
+  </si>
+  <si>
+    <t>[m2K/W] thermal contact resistance between soldi component, should be &gt;= 0; used if flag HTC_choice is 1</t>
+  </si>
+  <si>
+    <t>[m] Thickness of the interface between conductor components. For interfaces between components that are not both channels, assing in cell (comp1,comp2) the thickess of the interface of comp1  when in contact with comp2 and in cell  (comp2,comp1) the thickess of the interface of comp2  when in contact with comp1. Therefore the matrix may no longer be symmetric and also the lower triangular region should be filled.</t>
   </si>
 </sst>
 </file>
@@ -151,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -162,14 +166,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
@@ -182,23 +180,19 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -307,6 +301,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -553,27 +554,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -591,6 +571,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -608,7 +595,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CHAN"/>
@@ -628,7 +615,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="E3" t="str">
@@ -636,7 +623,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="3">
           <cell r="E3" t="str">
@@ -948,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631F8432-32B0-4782-8A41-3C8B7D94A95A}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -963,79 +950,79 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5" t="str">
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <f>[1]CHAN!E$3</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>[1]CHAN!F$3</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>[1]STR_MIX!E$3</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>[1]Z_JACKET!E$3</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1044,19 +1031,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1068,16 +1055,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1095,14 +1082,14 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="D4:F4 E5:F5 F6 C3 D3 E3 F3">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
-      <formula>1</formula>
+  <conditionalFormatting sqref="C3 D3:D4 E3:E5 F3:F6">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 D3 E3 F3 D4 E4 F4 E5 F5 F6">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="C3:F3 D4:F4 E5:F5 F6">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1111,6 +1098,193 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182F8F7F-A8D7-4239-AF85-1CCD06F5862A}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{11073E0C-B0B4-4CCC-ADAF-F7C7AD75C766}">
+            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{D8D42210-C82D-40ED-B579-6A74980D2860}">
+            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF3B1F8-15BE-471B-8C90-C91254905B72}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1134,54 +1308,54 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
@@ -1198,11 +1372,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1219,11 +1393,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1235,16 +1409,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1298,7 +1472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C628F5-9BDA-4746-9BD5-872CA60F8FA3}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1316,33 +1490,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="14" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="14" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="14" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="14" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
@@ -1363,7 +1537,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
@@ -1384,7 +1558,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
@@ -1405,7 +1579,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
@@ -1426,7 +1600,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
@@ -1442,7 +1616,7 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1471,80 +1645,80 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>0.009*PI()</f>
         <v>2.8274333882308135E-2</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1553,21 +1727,21 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f>3.7275</f>
         <v>3.7275</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f>0.094356</f>
         <v>9.4355999999999995E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1579,17 +1753,17 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f>0.031452</f>
         <v>3.1452000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1638,8 +1812,8 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{7A64B90D-B15C-4EB3-9FD8-4DB931DE61FC}">
-            <xm:f>contact_perimeter_flag!$F$6=0</xm:f>
+          <x14:cfRule type="expression" priority="5" id="{B5C1805D-6E53-462B-AAD2-E2CC9FC6C49C}">
+            <xm:f>contact_perimeter_flag!$E$4=0</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1648,8 +1822,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="12" id="{E2A6AA9F-F18E-4811-8631-F332CF0E94DA}">
-            <xm:f>contact_perimeter_flag!$F$6=1</xm:f>
+          <x14:cfRule type="expression" priority="6" id="{5DD1F1CF-914E-405F-A3AD-66002F6F60B9}">
+            <xm:f>contact_perimeter_flag!$E$4=1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1658,7 +1832,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F6</xm:sqref>
+          <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{092E39D0-6E06-4419-A5FC-56E43777B02C}">
@@ -1684,6 +1858,29 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{ABF31561-BDFE-4773-99F9-B8B63EB968DE}">
+            <xm:f>contact_perimeter_flag!$F$4=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{D46E27D2-07B7-4A9E-9EC4-1CCE139B18A6}">
+            <xm:f>contact_perimeter_flag!$F$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{6C12180F-7DA2-41FF-8849-9A5F5D212C8C}">
             <xm:f>contact_perimeter_flag!$F$5=0</xm:f>
             <x14:dxf>
@@ -1707,8 +1904,8 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{B5C1805D-6E53-462B-AAD2-E2CC9FC6C49C}">
-            <xm:f>contact_perimeter_flag!$E$4=0</xm:f>
+          <x14:cfRule type="expression" priority="11" id="{7A64B90D-B15C-4EB3-9FD8-4DB931DE61FC}">
+            <xm:f>contact_perimeter_flag!$F$6=0</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1717,8 +1914,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{5DD1F1CF-914E-405F-A3AD-66002F6F60B9}">
-            <xm:f>contact_perimeter_flag!$E$4=1</xm:f>
+          <x14:cfRule type="expression" priority="12" id="{E2A6AA9F-F18E-4811-8631-F332CF0E94DA}">
+            <xm:f>contact_perimeter_flag!$F$6=1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1727,30 +1924,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{ABF31561-BDFE-4773-99F9-B8B63EB968DE}">
-            <xm:f>contact_perimeter_flag!$F$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{D46E27D2-07B7-4A9E-9EC4-1CCE139B18A6}">
-            <xm:f>contact_perimeter_flag!$F$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F4</xm:sqref>
+          <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1776,105 +1950,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="103.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
         <v>-2</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
         <v>-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1883,19 +2057,19 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1909,7 +2083,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1970,6 +2144,29 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{D87FE0B6-C279-4964-A10A-104CDED6B425}">
+            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="6" id="{1A893477-A40F-4F07-B1C4-F0D1FD97855D}">
+            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="8" id="{A394923D-6402-4FF1-AB40-820FC3698AA3}">
             <xm:f>contact_perimeter_flag!$F$4=0</xm:f>
             <x14:dxf>
@@ -1991,29 +2188,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>F4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{D87FE0B6-C279-4964-A10A-104CDED6B425}">
-            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{1A893477-A40F-4F07-B1C4-F0D1FD97855D}">
-            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{A321D2D0-DBA7-4493-A63B-028B0F6E8C5B}">
@@ -2086,80 +2260,80 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1000</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -2168,19 +2342,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -2192,16 +2366,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -2270,6 +2444,29 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{DD84A92E-4778-4CBC-A9E6-30A79A7B937D}">
+            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="6" id="{5BE80D1C-95C5-43B3-A669-205F67CC700E}">
+            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{339C733E-4718-4A19-9E71-68CE042E9F11}">
             <xm:f>contact_perimeter_flag!$F$4=0</xm:f>
             <x14:dxf>
@@ -2291,29 +2488,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>F4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{DD84A92E-4778-4CBC-A9E6-30A79A7B937D}">
-            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{5BE80D1C-95C5-43B3-A669-205F67CC700E}">
-            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{C6C7C688-E427-4187-9B20-ADF8F226F297}">
@@ -2368,6 +2542,160 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245F1B56-37FE-4FDF-8CBC-77997752DD63}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF123C-7F60-4807-AE29-ECD4FCE24EA7}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2386,80 +2714,80 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -2468,19 +2796,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -2492,16 +2820,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -2524,8 +2852,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{61C546F9-9991-419A-AF57-2C4058E3D71E}">
-            <xm:f>contact_perimeter_flag!$F$6=0</xm:f>
+          <x14:cfRule type="expression" priority="5" id="{17FDCBAB-F36D-4D4B-9C83-7ECBE4FB5223}">
+            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2534,8 +2862,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="12" id="{F730F5E4-0B2A-4176-8FE7-A5C990469D53}">
-            <xm:f>contact_perimeter_flag!$F$6=1</xm:f>
+          <x14:cfRule type="expression" priority="6" id="{BAEF16C0-0DC7-4D87-99FB-10CBAE393ED8}">
+            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2544,7 +2872,69 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F6</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{FC3ADE6C-3A3E-4CAA-8D23-FF667BCC8A7C}">
+            <xm:f>contact_perimeter_flag!$E$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="7" id="{F5966269-AC0C-42CC-8070-274E500EFEAB}">
+            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="8" id="{99108EF2-B024-4528-A3BD-3537B6BF1AA3}">
+            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{83CFDED0-3481-40F2-8E50-A3A5BABFE4E8}">
+            <xm:f>contact_perimeter_flag!$E$4=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E4:F4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{D32D2F30-1A83-408E-BFB7-64FC762DD369}">
+            <xm:f>contact_perimeter_flag!$F$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{979BDE00-7B4D-44FD-B0A0-DAC806A8693B}">
@@ -2570,8 +2960,8 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{F5966269-AC0C-42CC-8070-274E500EFEAB}">
-            <xm:f>contact_perimeter_flag!$E$5=0</xm:f>
+          <x14:cfRule type="expression" priority="11" id="{61C546F9-9991-419A-AF57-2C4058E3D71E}">
+            <xm:f>contact_perimeter_flag!$F$6=0</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2580,8 +2970,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="8" id="{99108EF2-B024-4528-A3BD-3537B6BF1AA3}">
-            <xm:f>contact_perimeter_flag!$E$5=1</xm:f>
+          <x14:cfRule type="expression" priority="12" id="{F730F5E4-0B2A-4176-8FE7-A5C990469D53}">
+            <xm:f>contact_perimeter_flag!$F$6=1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2590,76 +2980,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{17FDCBAB-F36D-4D4B-9C83-7ECBE4FB5223}">
-            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{BAEF16C0-0DC7-4D87-99FB-10CBAE393ED8}">
-            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{CF8ABA04-E72C-451D-A640-CDB9EC8CB7EF}">
-            <xm:f>contact_perimeter_flag!$E$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="4" id="{FC3ADE6C-3A3E-4CAA-8D23-FF667BCC8A7C}">
-            <xm:f>contact_perimeter_flag!$E$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{83CFDED0-3481-40F2-8E50-A3A5BABFE4E8}">
-            <xm:f>contact_perimeter_flag!$E$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{D32D2F30-1A83-408E-BFB7-64FC762DD369}">
-            <xm:f>contact_perimeter_flag!$F$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F4</xm:sqref>
+          <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2667,7 +2988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3796B9-F96C-4711-80D4-7A42D4E01861}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2685,33 +3006,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="14" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="14" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="14" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="14" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
@@ -2732,7 +3053,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
@@ -2753,7 +3074,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
@@ -2774,7 +3095,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
@@ -2795,7 +3116,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
@@ -2821,7 +3142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC21CE9-E767-48C8-97C0-B436E3F8B9DC}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2839,33 +3160,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="14" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="14" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="14" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="14" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
@@ -2886,7 +3207,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
@@ -2907,7 +3228,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
@@ -2928,7 +3249,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
@@ -2949,7 +3270,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
@@ -2974,7 +3295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B35E1EA-762F-42F4-ACD0-F98E1885F191}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2999,60 +3320,60 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>0.293</f>
         <v>0.29299999999999998</v>
       </c>
@@ -3064,17 +3385,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="1">
@@ -3085,11 +3406,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -3106,11 +3427,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -3161,191 +3482,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182F8F7F-A8D7-4239-AF85-1CCD06F5862A}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD57"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
-        <f>contact_perimeter_flag!B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="C2" s="5" t="str">
-        <f>contact_perimeter_flag!C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="D2" s="5" t="str">
-        <f>contact_perimeter_flag!D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="E2" s="5" t="str">
-        <f>contact_perimeter_flag!E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="F2" s="5" t="str">
-        <f>contact_perimeter_flag!F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
-        <f>B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
-        <f>C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1E-3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
-        <f>D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
-        <f>E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
-        <f>F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{11073E0C-B0B4-4CCC-ADAF-F7C7AD75C766}">
-            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{D8D42210-C82D-40ED-B579-6A74980D2860}">
-            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D4</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>